<commit_message>
Removed a few endpoints for log generation, only POST endpoints left.
</commit_message>
<xml_diff>
--- a/WindWings_Report_Template.xlsx
+++ b/WindWings_Report_Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="104" documentId="11_314C95AEC5AF2F7A061A9C20379E4733104F7113" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A5EC79A-9DE9-4DBF-A23A-42B9CD353138}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="11_314C95AEC5AF2F7A061A9C20379E4733104F7113" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A191C864-C17A-48BC-8F06-ED7216D6484A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -774,7 +774,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>